<commit_message>
bento arm 4 diagnosis 12
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800744E9-702D-43EA-9648-238B6209FED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B78460-B2B7-423F-BD37-859EA0958D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -42,15 +42,9 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Beagle'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`</t>
-  </si>
-  <si>
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Beagle']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>TabName</t>
   </si>
   <si>
@@ -61,6 +55,47 @@
   </si>
   <si>
     <t>TC01_Bento_Filter_Arm-A_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+WHERE s.study_acronym IN ["A"]  
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+WITH ss
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+WHERE s.study_acronym IN ["A"]  
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files</t>
   </si>
 </sst>
 </file>
@@ -432,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,13 +482,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -462,21 +497,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Samples and Files Tab to all tests
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B78460-B2B7-423F-BD37-859EA0958D23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5AD767-A7E8-4A74-9D26-0A1F3E7F4BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -96,6 +96,72 @@
 COUNT(DISTINCT samp) AS Samples,
 COUNT(DISTINCT lp) AS Assays,
 COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+WITH COLLECT(ss.study_subject_id) AS all_subjects
+MATCH (samp:sample)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+WHERE s.study_acronym IN ["A"]  
+WITH
+    distinct lp,
+    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
+    collect(distinct f.file_id) AS files,
+    samp, ss, s, p, all_subjects
+RETURN
+ samp.sample_id AS `Sample ID`,
+            ss.study_subject_id AS `Case ID`,
+            p.program_acronym AS `Program Code`,
+            s.study_acronym AS `Arm`,
+            ss.disease_subtype AS `Diagnosis`,
+            samp.tissue_type AS `Tissue Type`,
+            samp.composition AS `Tissue Composition`,
+            samp.sample_anatomic_site AS `Sample Anatomic Site`,
+            samp.method_of_sample_procurement AS `Sample Procurement Method`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+WHERE s.study_acronym IN ["A"]  
+WITH
+        f, parent,p, ss, d,tp, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent,p, ss, d,tp, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent,p, ss, d,tp, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN Distinct
+    f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+     CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`
+    order by f.file_name</t>
   </si>
 </sst>
 </file>
@@ -465,22 +531,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="128.54296875" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -497,7 +563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -511,6 +577,40 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Bento 80 Test scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Arm-A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5AD767-A7E8-4A74-9D26-0A1F3E7F4BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE20FE32-54F4-4172-98BB-E8683947961A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,31 @@
   </si>
   <si>
     <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+WITH ss
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+WHERE s.study_acronym IN ["A"]  
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
@@ -76,32 +101,7 @@
        d.er_status AS `ER Status`,
        d.pr_status AS `PR Status`,
        demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WITH ss
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
-MATCH (samp)&lt;-[:file_of_sample]-(f)
-MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
-WHERE s.study_acronym IN ["A"]  
-RETURN COUNT(DISTINCT p) AS Programs,
-COUNT(DISTINCT s) AS Arms,
-COUNT(DISTINCT ss) AS Cases,
-COUNT(DISTINCT samp) AS Samples,
-COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
-  </si>
-  <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
+demo.survival_time AS `Survival (days)` Order By ss.study_subject_id ASC LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -127,7 +127,7 @@
             samp.tissue_type AS `Tissue Type`,
             samp.composition AS `Tissue Composition`,
             samp.sample_anatomic_site AS `Sample Anatomic Site`,
-            samp.method_of_sample_procurement AS `Sample Procurement Method`</t>
+            samp.method_of_sample_procurement AS `Sample Procurement Method` Order By samp.sample_id ASC LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -161,7 +161,7 @@
     s.study_acronym AS `Arm`,
     ss.study_subject_id AS `Case ID`,
     samp.sample_id AS `Sample ID`
-    order by f.file_name</t>
+ order By f.file_name ASC LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,10 +568,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -580,15 +580,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="360" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -599,13 +599,13 @@
     </row>
     <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>

</xml_diff>